<commit_message>
Updates on 18 Nov 2020
</commit_message>
<xml_diff>
--- a/TheMasterProject/Content/DocBook1.xlsx
+++ b/TheMasterProject/Content/DocBook1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kpmgindia365-my.sharepoint.com/personal/sunnykumar3_kpmg_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunnykumar3\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E69A6BF7-9EE1-40B9-A8E1-2EE6C980B6CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDD02B7D-6925-46C2-957E-B92649360D97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{41EAC47F-9EB0-45E0-9900-5EDE14FD3CBF}"/>
+    <workbookView xWindow="3855" yWindow="525" windowWidth="15375" windowHeight="7875" xr2:uid="{224DF3B9-9E70-4271-ABAA-39CB64A93354}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>BuyerName</t>
   </si>
@@ -40,6 +42,12 @@
   </si>
   <si>
     <t>Sarita</t>
+  </si>
+  <si>
+    <t>Mohit</t>
+  </si>
+  <si>
+    <t>Pandey</t>
   </si>
 </sst>
 </file>
@@ -390,11 +398,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650BA342-70AD-4063-8F6F-E57D81B19709}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B21FF5-30F3-4025-B7F6-4993B52B52F5}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,283 +423,23 @@
         <v>88876</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>77778</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>777654</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A77AFFAB4340884AA52D23997744F00F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8dac9d3e12a3c932194b05dd0857993d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="485a6337-a3da-48ee-9628-b8b655699cae" xmlns:ns4="0e241b5f-2e33-498b-ae99-32a4be288059" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e73b77b2a043383b3a4e7b435301ef5" ns3:_="" ns4:_="">
-    <xsd:import namespace="485a6337-a3da-48ee-9628-b8b655699cae"/>
-    <xsd:import namespace="0e241b5f-2e33-498b-ae99-32a4be288059"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceKeyPoints" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="485a6337-a3da-48ee-9628-b8b655699cae" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0e241b5f-2e33-498b-ae99-32a4be288059" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0561A1D-376A-404B-9297-4CB392260032}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="485a6337-a3da-48ee-9628-b8b655699cae"/>
-    <ds:schemaRef ds:uri="0e241b5f-2e33-498b-ae99-32a4be288059"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33393B2D-9597-46F8-A76F-CF73C6BD6DBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2CB508-BD77-4801-B598-85611907778E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0e241b5f-2e33-498b-ae99-32a4be288059"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="485a6337-a3da-48ee-9628-b8b655699cae"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>